<commit_message>
Added constant versions property
</commit_message>
<xml_diff>
--- a/utils/codata_units.xlsx
+++ b/utils/codata_units.xlsx
@@ -10,11 +10,11 @@
     <sheet state="visible" name="v2010" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="2" name="Z_EEDDD780_5E0E_4B3C_8FB2_945B1D76B546_.wvu.FilterData">'v2018'!$A$1:$D$355</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_1D2F3C64_6FDE_4D7D_BFC8_1FADDFDCA87B_.wvu.FilterData">'v2018'!$A$1:$D$355</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{EEDDD780-5E0E-4B3C-8FB2-945B1D76B546}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1D2F3C64-6FDE-4D7D-BFC8-1FADDFDCA87B}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -6839,7 +6839,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000000E+00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6877,10 +6877,6 @@
       <color rgb="FF666666"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <color rgb="FF999999"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -6896,7 +6892,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6922,9 +6918,6 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -30314,7 +30307,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{EEDDD780-5E0E-4B3C-8FB2-945B1D76B546}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{1D2F3C64-6FDE-4D7D-BFC8-1FADDFDCA87B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$D$355">
         <filterColumn colId="1">
           <customFilters>
@@ -30369,7 +30362,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3"/>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -45609,8 +45602,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">

</xml_diff>

<commit_message>
Added licenses to readme
</commit_message>
<xml_diff>
--- a/utils/codata_units.xlsx
+++ b/utils/codata_units.xlsx
@@ -10,11 +10,11 @@
     <sheet state="visible" name="v2010" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="2" name="Z_1D2F3C64_6FDE_4D7D_BFC8_1FADDFDCA87B_.wvu.FilterData">'v2018'!$A$1:$D$355</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_BB9B5AF0_0E9F_4252_8AEE_A0C2B3151743_.wvu.FilterData">'v2018'!$A$1:$D$355</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1D2F3C64-6FDE-4D7D-BFC8-1FADDFDCA87B}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{BB9B5AF0-0E9F-4252-8AEE-A0C2B3151743}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -30307,7 +30307,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1D2F3C64-6FDE-4D7D-BFC8-1FADDFDCA87B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{BB9B5AF0-0E9F-4252-8AEE-A0C2B3151743}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$D$355">
         <filterColumn colId="1">
           <customFilters>

</xml_diff>